<commit_message>
SS : Update all xlsx files to their new name MISC : Update RunHTTPServer script as for loop not working on chrome OS ?!
</commit_message>
<xml_diff>
--- a/Data/FiMs Pay.xlsx
+++ b/Data/FiMs Pay.xlsx
@@ -8,7 +8,9 @@
     <sheet state="visible" name="Pool" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Merchant" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Transactions!$A$1:$G$12</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="194">
   <si>
     <t>Type</t>
   </si>
@@ -25625,6 +25627,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.75"/>
+    <col customWidth="1" min="6" max="6" width="12.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -25652,10 +25655,10 @@
     </row>
     <row r="2">
       <c r="A2" s="11">
-        <v>44673.49886574074</v>
+        <v>44681.499131944445</v>
       </c>
       <c r="B2" s="12">
-        <v>7.26</v>
+        <v>3.5</v>
       </c>
       <c r="C2" s="4">
         <v>2.0</v>
@@ -25664,20 +25667,20 @@
         <v>170</v>
       </c>
       <c r="E2" s="4">
-        <v>7.84</v>
+        <v>3.69</v>
       </c>
       <c r="F2" s="13">
-        <f t="shared" ref="F2:F7" si="1">E2/B2</f>
-        <v>1.079889807</v>
+        <f t="shared" ref="F2:F12" si="1">E2/B2</f>
+        <v>1.054285714</v>
       </c>
       <c r="G2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="11">
-        <v>44672.5059837963</v>
+        <v>44680.53349537037</v>
       </c>
       <c r="B3" s="12">
-        <v>4.18</v>
+        <v>10.8</v>
       </c>
       <c r="C3" s="4">
         <v>2.0</v>
@@ -25686,20 +25689,20 @@
         <v>170</v>
       </c>
       <c r="E3" s="4">
-        <v>4.56</v>
+        <v>11.41</v>
       </c>
       <c r="F3" s="13">
         <f t="shared" si="1"/>
-        <v>1.090909091</v>
+        <v>1.056481481</v>
       </c>
       <c r="G3" s="13"/>
     </row>
     <row r="4">
       <c r="A4" s="11">
-        <v>44667.50069444445</v>
+        <v>44679.53175925926</v>
       </c>
       <c r="B4" s="12">
-        <v>3.5</v>
+        <v>5.9</v>
       </c>
       <c r="C4" s="4">
         <v>2.0</v>
@@ -25708,20 +25711,20 @@
         <v>170</v>
       </c>
       <c r="E4" s="4">
-        <v>3.78</v>
+        <v>6.2</v>
       </c>
       <c r="F4" s="13">
         <f t="shared" si="1"/>
-        <v>1.08</v>
+        <v>1.050847458</v>
       </c>
       <c r="G4" s="13"/>
     </row>
     <row r="5">
       <c r="A5" s="11">
-        <v>44666.53603009259</v>
+        <v>44675.52208333334</v>
       </c>
       <c r="B5" s="12">
-        <v>14.1</v>
+        <v>3.5</v>
       </c>
       <c r="C5" s="4">
         <v>2.0</v>
@@ -25730,20 +25733,20 @@
         <v>170</v>
       </c>
       <c r="E5" s="4">
-        <v>15.24</v>
+        <v>3.78</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="1"/>
-        <v>1.080851064</v>
+        <v>1.08</v>
       </c>
       <c r="G5" s="13"/>
     </row>
     <row r="6">
       <c r="A6" s="11">
-        <v>44665.4934375</v>
+        <v>44674.54173611111</v>
       </c>
       <c r="B6" s="12">
-        <v>6.55</v>
+        <v>4.8</v>
       </c>
       <c r="C6" s="4">
         <v>2.0</v>
@@ -25752,20 +25755,20 @@
         <v>170</v>
       </c>
       <c r="E6" s="4">
-        <v>7.15</v>
+        <v>5.18</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="1"/>
-        <v>1.091603053</v>
+        <v>1.079166667</v>
       </c>
       <c r="G6" s="13"/>
     </row>
     <row r="7">
       <c r="A7" s="11">
-        <v>44660.44101851852</v>
-      </c>
-      <c r="B7" s="14">
-        <v>3.0</v>
+        <v>44673.49886574074</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7.26</v>
       </c>
       <c r="C7" s="4">
         <v>2.0</v>
@@ -25774,15 +25777,126 @@
         <v>170</v>
       </c>
       <c r="E7" s="4">
+        <v>7.84</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="1"/>
+        <v>1.079889807</v>
+      </c>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11">
+        <v>44672.5059837963</v>
+      </c>
+      <c r="B8" s="12">
+        <v>4.18</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4.56</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>1.090909091</v>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="11">
+        <v>44667.50069444445</v>
+      </c>
+      <c r="B9" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3.78</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="1"/>
+        <v>1.08</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="11">
+        <v>44666.53603009259</v>
+      </c>
+      <c r="B10" s="12">
+        <v>14.1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="4">
+        <v>15.24</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="1"/>
+        <v>1.080851064</v>
+      </c>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="11">
+        <v>44665.4934375</v>
+      </c>
+      <c r="B11" s="12">
+        <v>6.55</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="4">
+        <v>7.15</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="1"/>
+        <v>1.091603053</v>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="11">
+        <v>44660.524351851855</v>
+      </c>
+      <c r="B12" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="4">
         <v>3.26</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F12" s="13">
         <f t="shared" si="1"/>
         <v>1.086666667</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$G$12"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -25822,8 +25936,8 @@
     </row>
     <row r="2">
       <c r="A2" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTXML(""https://www.xe.com/en/currencyconverter/convert/?Amount=1000&amp;From=EUR&amp;To=USD"",""//p[@class='result__BigRate-sc-1bsijpp-1 iGrAod']"")/1000"),1.07954)</f>
-        <v>1.07954</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTXML(""https://www.xe.com/en/currencyconverter/convert/?Amount=1000&amp;From=EUR&amp;To=USD"",""//p[@class='result__BigRate-sc-1bsijpp-1 iGrAod']"")/1000"),1.0544200000000001)</f>
+        <v>1.05442</v>
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:C2" si="1">SUM(OFFSET(B:B,ROW(),0))</f>
@@ -25974,7 +26088,7 @@
       </c>
       <c r="L2" s="17">
         <f>SUMIFS(Transactions!$B:$B,Transactions!$C:$C,$A2,Transactions!$G:$G,"")</f>
-        <v>38.59</v>
+        <v>67.09</v>
       </c>
       <c r="M2" s="18">
         <f t="shared" ref="M2:N2" si="1">SWITCH(H2,"Monthly",DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),"Weekly",TODAY()+7-WEEKDAY(TODAY(),2),"Daily",TODAY())</f>
@@ -25982,7 +26096,7 @@
       </c>
       <c r="N2" s="18">
         <f t="shared" si="1"/>
-        <v>44675</v>
+        <v>44682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SS : Remove sensible associate data from spreadsheet SCRIPT : Start the web browser with a user ID input by a user SCRIPT : Add a Download All spreadsheet option SCRIPT : Use associative array to factorise (only in shell) SS : Update all spreadsheet MISC : Update ReadMe.md
</commit_message>
<xml_diff>
--- a/Data/FiMs Pay.xlsx
+++ b/Data/FiMs Pay.xlsx
@@ -5,11 +5,12 @@
   <sheets>
     <sheet state="hidden" name="Solflare activity" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Transactions" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Pool" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Merchant" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Merchant" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Pool" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="PaidTransactions" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Transactions!$A$1:$G$12</definedName>
+    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">PaidTransactions!$A$1:$F$21</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="192">
   <si>
     <t>Type</t>
   </si>
@@ -658,79 +659,73 @@
     <t>Change rate</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Crypto Address</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Not Paid</t>
+  </si>
+  <si>
     <t>Paid</t>
   </si>
   <si>
-    <t>UST</t>
+    <t>Next withdraw</t>
+  </si>
+  <si>
+    <t>lepaindannette@free.fr</t>
+  </si>
+  <si>
+    <t>SARL Le pain d'Annette</t>
+  </si>
+  <si>
+    <t>FR76 1380 7001 4232 4212 1064 671</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>contact@natureetbulles.com</t>
+  </si>
+  <si>
+    <t>Nature et bulles</t>
+  </si>
+  <si>
+    <t>FR76 1290 6000 1557 4515 0307 551</t>
   </si>
   <si>
     <t>EUR</t>
   </si>
   <si>
+    <t>Currency</t>
+  </si>
+  <si>
     <t>Change Rate</t>
   </si>
   <si>
-    <t>Person</t>
+    <t>agEUR</t>
   </si>
   <si>
-    <t>Bloopsy</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Company IBAN</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Personal IBAN</t>
-  </si>
-  <si>
-    <t>Withdraw</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Not Paid</t>
-  </si>
-  <si>
-    <t>Next withdraw</t>
-  </si>
-  <si>
-    <t>Next report</t>
-  </si>
-  <si>
-    <t>SARL Le pain d'Annette</t>
-  </si>
-  <si>
-    <t>FR7613807001423242121064671</t>
-  </si>
-  <si>
-    <t>Anne Labrosse</t>
-  </si>
-  <si>
-    <t>FR7613807001423291914331236</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>Weekly</t>
-  </si>
-  <si>
-    <t>lepaindannette@free.fr</t>
+    <t>UST</t>
   </si>
 </sst>
 </file>
@@ -769,7 +764,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,6 +781,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA4C2F4"/>
         <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -805,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -844,15 +845,26 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="169" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="170" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -887,6 +899,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -25649,259 +25665,165 @@
       <c r="F1" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="11">
-        <v>44681.499131944445</v>
-      </c>
-      <c r="B2" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="4">
-        <v>3.69</v>
-      </c>
-      <c r="F2" s="13">
-        <f t="shared" ref="F2:F12" si="1">E2/B2</f>
-        <v>1.054285714</v>
-      </c>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="11">
-        <v>44680.53349537037</v>
-      </c>
-      <c r="B3" s="12">
-        <v>10.8</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="4">
-        <v>11.41</v>
-      </c>
-      <c r="F3" s="13">
-        <f t="shared" si="1"/>
-        <v>1.056481481</v>
-      </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="11">
-        <v>44679.53175925926</v>
-      </c>
-      <c r="B4" s="12">
-        <v>5.9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" s="4">
-        <v>6.2</v>
-      </c>
-      <c r="F4" s="13">
-        <f t="shared" si="1"/>
-        <v>1.050847458</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="11">
-        <v>44675.52208333334</v>
-      </c>
-      <c r="B5" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.78</v>
-      </c>
-      <c r="F5" s="13">
-        <f t="shared" si="1"/>
-        <v>1.08</v>
-      </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="11">
-        <v>44674.54173611111</v>
-      </c>
-      <c r="B6" s="12">
-        <v>4.8</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5.18</v>
-      </c>
-      <c r="F6" s="13">
-        <f t="shared" si="1"/>
-        <v>1.079166667</v>
-      </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11">
-        <v>44673.49886574074</v>
-      </c>
-      <c r="B7" s="12">
-        <v>7.26</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="4">
-        <v>7.84</v>
-      </c>
-      <c r="F7" s="13">
-        <f t="shared" si="1"/>
-        <v>1.079889807</v>
-      </c>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="11">
-        <v>44672.5059837963</v>
-      </c>
-      <c r="B8" s="12">
-        <v>4.18</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E8" s="4">
-        <v>4.56</v>
-      </c>
-      <c r="F8" s="13">
-        <f t="shared" si="1"/>
-        <v>1.090909091</v>
-      </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="11">
-        <v>44667.50069444445</v>
-      </c>
-      <c r="B9" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="4">
-        <v>3.78</v>
-      </c>
-      <c r="F9" s="13">
-        <f t="shared" si="1"/>
-        <v>1.08</v>
-      </c>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="11">
-        <v>44666.53603009259</v>
-      </c>
-      <c r="B10" s="12">
-        <v>14.1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E10" s="4">
-        <v>15.24</v>
-      </c>
-      <c r="F10" s="13">
-        <f t="shared" si="1"/>
-        <v>1.080851064</v>
-      </c>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="11">
-        <v>44665.4934375</v>
-      </c>
-      <c r="B11" s="12">
-        <v>6.55</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="4">
-        <v>7.15</v>
-      </c>
-      <c r="F11" s="13">
-        <f t="shared" si="1"/>
-        <v>1.091603053</v>
-      </c>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="11">
-        <v>44660.524351851855</v>
-      </c>
-      <c r="B12" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3.26</v>
-      </c>
-      <c r="F12" s="13">
-        <f t="shared" si="1"/>
-        <v>1.086666667</v>
-      </c>
-      <c r="G12" s="13"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$G$12"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="2.63"/>
+    <col customWidth="1" min="2" max="2" width="17.38"/>
+    <col customWidth="1" min="3" max="3" width="18.25"/>
+    <col customWidth="1" min="4" max="4" width="28.0"/>
+    <col customWidth="1" min="5" max="5" width="5.13"/>
+    <col customWidth="1" min="6" max="6" width="25.0"/>
+    <col customWidth="1" min="7" max="7" width="4.38"/>
+    <col customWidth="1" min="8" max="11" width="10.13"/>
+    <col customWidth="1" min="12" max="12" width="12.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <f t="shared" ref="A2:A3" si="1">ROW()</f>
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="16">
+        <f t="shared" ref="G2:G3" si="2">1-E2</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="17">
+        <f>SUMIFS(Transactions!$B:$B,Transactions!$C:$C,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="18">
+        <f>SUMIFS(PaidTransactions!$B:$B,PaidTransactions!$C:$C,$A2)</f>
+        <v>110.09</v>
+      </c>
+      <c r="L2" s="19">
+        <f t="shared" ref="L2:L3" si="3">SWITCH(H2,"Monthly",DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),"Weekly",TODAY()+7-WEEKDAY(TODAY(),2),"Daily",TODAY())</f>
+        <v>44703</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="17">
+        <f>SUMIFS(Transactions!$B:$B,Transactions!$C:$C,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="18">
+        <f>SUMIFS(PaidTransactions!$B:$B,PaidTransactions!$C:$C,$A3)</f>
+        <v>29</v>
+      </c>
+      <c r="L3" s="19">
+        <f t="shared" si="3"/>
+        <v>44703</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -25922,53 +25844,89 @@
         <v>163</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTXML(""https://www.xe.com/en/currencyconverter/convert/?Amount=1000&amp;From=EUR&amp;To=USD"",""//p[@class='result__BigRate-sc-1bsijpp-1 iGrAod']"")/1000"),1.0544200000000001)</f>
-        <v>1.05442</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTXML(""https://www.xe.com/en/currencyconverter/convert/?Amount=1000&amp;From=EUR&amp;To=USD"",""//p[@class='result__BigRate-sc-1bsijpp-1 iGrAod']"")/1000"),1.0478599999999998)</f>
+        <v>1.04786</v>
       </c>
       <c r="B2" s="9">
-        <f t="shared" ref="B2:C2" si="1">SUM(OFFSET(B:B,ROW(),0))</f>
-        <v>100</v>
-      </c>
-      <c r="C2" s="9">
-        <f t="shared" si="1"/>
-        <v>-108.98734</v>
-      </c>
+        <f>SUM(OFFSET(B:B,ROW(),0))</f>
+        <v>180</v>
+      </c>
+      <c r="C2" s="9"/>
       <c r="D2" s="9">
-        <f>AVERAGE(OFFSET(D:D,ROW(),0))</f>
-        <v>1.0898734</v>
-      </c>
-      <c r="E2" s="9"/>
+        <f>SUM(OFFSET(D:D,ROW(),0))</f>
+        <v>-188.98734</v>
+      </c>
+      <c r="E2" s="9">
+        <f>AVERAGE(OFFSET(E:E,ROW(),0))</f>
+        <v>1.0299578</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="11">
+        <v>44691.71973379629</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-45.0</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E5" si="1">-D3/B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11">
+        <v>44687.69899305556</v>
+      </c>
+      <c r="B4" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-35.0</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11">
         <v>44657.928136574075</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B5" s="4">
         <v>100.0</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="20">
         <v>-108.98734</v>
       </c>
-      <c r="D3" s="7">
-        <f>-C3/B3</f>
+      <c r="E5" s="7">
+        <f t="shared" si="1"/>
         <v>1.0898734</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -25976,7 +25934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -25989,117 +25947,432 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.63"/>
-    <col customWidth="1" min="2" max="2" width="18.25"/>
-    <col customWidth="1" min="3" max="3" width="25.0"/>
-    <col customWidth="1" min="4" max="4" width="5.13"/>
-    <col customWidth="1" min="5" max="5" width="11.88"/>
-    <col customWidth="1" min="6" max="6" width="25.0"/>
-    <col customWidth="1" min="7" max="7" width="4.38"/>
-    <col customWidth="1" min="8" max="8" width="8.25"/>
-    <col customWidth="1" min="9" max="9" width="6.75"/>
-    <col customWidth="1" min="10" max="10" width="17.38"/>
-    <col customWidth="1" min="11" max="11" width="5.5"/>
-    <col customWidth="1" min="12" max="12" width="7.63"/>
-    <col customWidth="1" min="13" max="13" width="11.88"/>
-    <col customWidth="1" min="14" max="14" width="11.5"/>
+    <col customWidth="1" min="1" max="1" width="15.75"/>
+    <col customWidth="1" min="6" max="6" width="12.75"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>186</v>
+        <v>167</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
-        <f>ROW()</f>
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="A2" s="11">
+        <v>44691.72447916667</v>
+      </c>
+      <c r="B2" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="C2" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="21">
+        <v>12.0</v>
+      </c>
+      <c r="F2" s="13">
         <v>1.0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2" s="4" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="11">
+        <v>44695.55331018519</v>
+      </c>
+      <c r="B3" s="12">
+        <v>5.4</v>
+      </c>
+      <c r="C3" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="G2" s="16">
-        <f>1-D2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="E3" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11">
+        <v>44693.51792824074</v>
+      </c>
+      <c r="B4" s="12">
+        <v>8.1</v>
+      </c>
+      <c r="C4" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="21">
+        <v>8.1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11">
+        <v>44687.533043981486</v>
+      </c>
+      <c r="B5" s="12">
+        <v>6.6</v>
+      </c>
+      <c r="C5" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="21">
+        <v>6.6</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11">
+        <v>44687.83658564815</v>
+      </c>
+      <c r="B6" s="12">
+        <v>17.0</v>
+      </c>
+      <c r="C6" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="21">
+        <v>17.0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11">
+        <v>44689.50938657408</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7.3</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="21">
+        <v>7.3</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11">
+        <v>44688.54746527778</v>
+      </c>
+      <c r="B8" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11">
+        <v>44686.46728009259</v>
+      </c>
+      <c r="B9" s="12">
+        <v>7.1</v>
+      </c>
+      <c r="C9" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" s="21">
+        <v>7.1</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11">
+        <v>44686.52086805555</v>
+      </c>
+      <c r="B10" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11">
+        <v>44681.499131944445</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C11" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="K2" s="17">
-        <f>SUMIFS(Transactions!$B:$B,Transactions!$C:$C,$A2,Transactions!$G:$G,"&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="17">
-        <f>SUMIFS(Transactions!$B:$B,Transactions!$C:$C,$A2,Transactions!$G:$G,"")</f>
-        <v>67.09</v>
-      </c>
-      <c r="M2" s="18">
-        <f t="shared" ref="M2:N2" si="1">SWITCH(H2,"Monthly",DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),"Weekly",TODAY()+7-WEEKDAY(TODAY(),2),"Daily",TODAY())</f>
-        <v>44682</v>
-      </c>
-      <c r="N2" s="18">
-        <f t="shared" si="1"/>
-        <v>44682</v>
+      <c r="E11" s="21">
+        <v>3.69</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1.0542857142857143</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11">
+        <v>44680.53349537037</v>
+      </c>
+      <c r="B12" s="12">
+        <v>10.8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="21">
+        <v>11.41</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1.0564814814814814</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11">
+        <v>44679.53175925926</v>
+      </c>
+      <c r="B13" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="C13" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="21">
+        <v>6.2</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1.0508474576271185</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11">
+        <v>44675.52208333333</v>
+      </c>
+      <c r="B14" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C14" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="21">
+        <v>3.78</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1.0799999999999998</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11">
+        <v>44674.54173611111</v>
+      </c>
+      <c r="B15" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="C15" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="21">
+        <v>5.18</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1.0791666666666666</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11">
+        <v>44673.49886574074</v>
+      </c>
+      <c r="B16" s="12">
+        <v>7.26</v>
+      </c>
+      <c r="C16" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="21">
+        <v>7.84</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1.0798898071625345</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11">
+        <v>44672.5059837963</v>
+      </c>
+      <c r="B17" s="12">
+        <v>4.18</v>
+      </c>
+      <c r="C17" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="21">
+        <v>4.56</v>
+      </c>
+      <c r="F17" s="13">
+        <v>1.0909090909090908</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11">
+        <v>44667.50069444445</v>
+      </c>
+      <c r="B18" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="21">
+        <v>3.78</v>
+      </c>
+      <c r="F18" s="13">
+        <v>1.0799999999999998</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11">
+        <v>44666.5360300926</v>
+      </c>
+      <c r="B19" s="12">
+        <v>14.1</v>
+      </c>
+      <c r="C19" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="21">
+        <v>15.24</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1.0808510638297872</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11">
+        <v>44665.4934375</v>
+      </c>
+      <c r="B20" s="12">
+        <v>6.55</v>
+      </c>
+      <c r="C20" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="21">
+        <v>7.15</v>
+      </c>
+      <c r="F20" s="13">
+        <v>1.0916030534351147</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11">
+        <v>44660.524351851855</v>
+      </c>
+      <c r="B21" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C21" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="21">
+        <v>3.26</v>
+      </c>
+      <c r="F21" s="13">
+        <v>1.0866666666666667</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$F$21"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>